<commit_message>
see update in README
</commit_message>
<xml_diff>
--- a/robot-wiring.xlsx
+++ b/robot-wiring.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>wiring</t>
   </si>
@@ -58,6 +58,51 @@
   </si>
   <si>
     <t xml:space="preserve">lynxmotion rx(robot arm) </t>
+  </si>
+  <si>
+    <t>rx0</t>
+  </si>
+  <si>
+    <t>tx1</t>
+  </si>
+  <si>
+    <t>tx3</t>
+  </si>
+  <si>
+    <t>rx3</t>
+  </si>
+  <si>
+    <t>tx2</t>
+  </si>
+  <si>
+    <t>rx2</t>
+  </si>
+  <si>
+    <t>rx1</t>
+  </si>
+  <si>
+    <t>sda</t>
+  </si>
+  <si>
+    <t>scl</t>
+  </si>
+  <si>
+    <t>SCL(LCD)</t>
+  </si>
+  <si>
+    <t>SDA(LCD)</t>
+  </si>
+  <si>
+    <t>rasp pi (rx)</t>
+  </si>
+  <si>
+    <t>rasp pi (tx)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trig back sonar </t>
+  </si>
+  <si>
+    <t>echo back sonar</t>
   </si>
 </sst>
 </file>
@@ -396,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -416,16 +461,25 @@
       <c r="A2">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
       <c r="C4" t="s">
         <v>1</v>
       </c>
@@ -437,6 +491,9 @@
       <c r="A5">
         <v>3</v>
       </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
       <c r="C5" t="s">
         <v>1</v>
       </c>
@@ -448,6 +505,9 @@
       <c r="A6">
         <v>4</v>
       </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
       <c r="C6" t="s">
         <v>1</v>
       </c>
@@ -459,6 +519,9 @@
       <c r="A7">
         <v>5</v>
       </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
       <c r="C7" t="s">
         <v>1</v>
       </c>
@@ -470,6 +533,9 @@
       <c r="A8">
         <v>6</v>
       </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
@@ -478,6 +544,9 @@
       <c r="A9">
         <v>7</v>
       </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
       <c r="C9" t="s">
         <v>7</v>
       </c>
@@ -486,6 +555,9 @@
       <c r="A10">
         <v>8</v>
       </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
       <c r="C10" t="s">
         <v>8</v>
       </c>
@@ -494,6 +566,9 @@
       <c r="A11">
         <v>9</v>
       </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
       <c r="C11" t="s">
         <v>9</v>
       </c>
@@ -502,6 +577,9 @@
       <c r="A12">
         <v>10</v>
       </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
       <c r="C12" t="s">
         <v>10</v>
       </c>
@@ -510,6 +588,9 @@
       <c r="A13">
         <v>11</v>
       </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
       <c r="C13" t="s">
         <v>11</v>
       </c>
@@ -518,16 +599,31 @@
       <c r="A14">
         <v>12</v>
       </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
+      <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
       <c r="C16" t="s">
         <v>12</v>
       </c>
@@ -536,23 +632,71 @@
       <c r="A17">
         <v>15</v>
       </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
       <c r="C20" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update wiring csv and mainBot code
</commit_message>
<xml_diff>
--- a/robot-wiring.xlsx
+++ b/robot-wiring.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>wiring</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>echo back sonar</t>
+  </si>
+  <si>
+    <t>yellow</t>
   </si>
 </sst>
 </file>
@@ -444,7 +447,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -626,6 +629,9 @@
       </c>
       <c r="C16" t="s">
         <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update wiring, added sonarOffset model
</commit_message>
<xml_diff>
--- a/robot-wiring.xlsx
+++ b/robot-wiring.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\datng\OneDrive\pPlayground\arduino\project\unlRobotic2018\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="18" documentId="11_32807BF66E22D1C743F6E2BD690367C79DA336A6" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{2F0E7702-7369-49C2-8CC8-109979C6C384}"/>
   <bookViews>
-    <workbookView xWindow="192" yWindow="108" windowWidth="7620" windowHeight="4512"/>
+    <workbookView xWindow="192" yWindow="108" windowWidth="7620" windowHeight="4512" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>wiring</t>
   </si>
@@ -42,18 +48,6 @@
     <t>CA_Shoulder</t>
   </si>
   <si>
-    <t>trig left sonar</t>
-  </si>
-  <si>
-    <t>echo left sonar</t>
-  </si>
-  <si>
-    <t>trig right sonar</t>
-  </si>
-  <si>
-    <t>echo right sonar</t>
-  </si>
-  <si>
     <t xml:space="preserve">sabertooth(encoder Driver) rx </t>
   </si>
   <si>
@@ -99,19 +93,37 @@
     <t>rasp pi (tx)</t>
   </si>
   <si>
-    <t xml:space="preserve">trig back sonar </t>
-  </si>
-  <si>
-    <t>echo back sonar</t>
-  </si>
-  <si>
     <t>yellow</t>
+  </si>
+  <si>
+    <t>left trig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">left echo </t>
+  </si>
+  <si>
+    <t>right trig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">right echo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">back trig </t>
+  </si>
+  <si>
+    <t xml:space="preserve">back echo </t>
+  </si>
+  <si>
+    <t>front trig</t>
+  </si>
+  <si>
+    <t>front echo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -152,6 +164,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -200,7 +215,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -233,9 +248,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -268,6 +300,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -443,40 +492,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="3" max="4" width="26.109375" customWidth="1"/>
+    <col min="3" max="4" width="26.1015625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>2</v>
       </c>
@@ -490,7 +539,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>3</v>
       </c>
@@ -504,7 +553,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>4</v>
       </c>
@@ -518,7 +567,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>5</v>
       </c>
@@ -532,7 +581,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>6</v>
       </c>
@@ -543,7 +592,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>7</v>
       </c>
@@ -554,155 +603,188 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11">
-        <v>9</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14">
-        <v>12</v>
-      </c>
-      <c r="C14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15">
-        <v>13</v>
-      </c>
-      <c r="C15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24">
         <v>22</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25">
         <v>23</v>
+      </c>
+      <c r="C25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="C26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="C27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="C28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="C29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="C30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="C31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -711,24 +793,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>